<commit_message>
requesitos e especificação atualizadas
</commit_message>
<xml_diff>
--- a/2ª Fase/Diagramas/Especificaçao.xlsx
+++ b/2ª Fase/Diagramas/Especificaçao.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="8445" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="8445" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Procurar restaurante" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="113">
   <si>
     <t>Name</t>
   </si>
@@ -454,9 +454,6 @@
     <t>Escolhe negócio</t>
   </si>
   <si>
-    <t>Preenche pontuação e campos obrigatórios</t>
-  </si>
-  <si>
     <t>Guarda dados</t>
   </si>
   <si>
@@ -489,9 +486,6 @@
     <t>Volta a 3</t>
   </si>
   <si>
-    <t>Adiciona aos favoritos</t>
-  </si>
-  <si>
     <t>Permite ao utilizador adicionar um restaurante aos favoritos</t>
   </si>
   <si>
@@ -637,6 +631,67 @@
   </si>
   <si>
     <t>Não confirma</t>
+  </si>
+  <si>
+    <t>Volta para 8</t>
+  </si>
+  <si>
+    <t>Seleciona etiqueta e adiciona aos favoritos</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Comportamento Alternativo 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(passo 16)</t>
+    </r>
+  </si>
+  <si>
+    <t>Volta para 16</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Comportamento Alternativo 3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(passo 16)</t>
+    </r>
+  </si>
+  <si>
+    <t>Preenche pontuação e critica</t>
+  </si>
+  <si>
+    <t>Escolhe negócio e ementa consumida</t>
   </si>
 </sst>
 </file>
@@ -819,6 +874,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -840,19 +907,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1150,58 +1205,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -1521,58 +1576,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -1592,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -1603,7 +1658,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -1612,7 +1667,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -1623,7 +1678,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -1632,7 +1687,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E13" s="4"/>
     </row>
@@ -1653,7 +1708,7 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -1662,7 +1717,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
@@ -1703,74 +1758,74 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="17" t="s">
-        <v>97</v>
+      <c r="B22" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="20">
+      <c r="C23" s="12">
         <v>2</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20" t="s">
-        <v>98</v>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="17"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="17"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
@@ -1850,58 +1905,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -1921,7 +1976,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -1932,7 +1987,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -1941,7 +1996,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -1952,7 +2007,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -1961,7 +2016,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E13" s="4"/>
     </row>
@@ -1972,7 +2027,7 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1988,7 +2043,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
@@ -2029,74 +2084,74 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="17" t="s">
-        <v>106</v>
+      <c r="B22" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="20">
+      <c r="C23" s="12">
         <v>2</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20" t="s">
-        <v>88</v>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="17"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="17"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
@@ -2163,8 +2218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,58 +2231,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -2393,21 +2448,21 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="9">
-        <v>1</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="C24" s="4">
+        <v>16</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="4">
+        <v>17</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
@@ -2417,61 +2472,61 @@
     </row>
     <row r="27" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C27" s="9">
         <v>1</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="9"/>
+      <c r="E29" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="9">
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="9">
         <v>2</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9" t="s">
+      <c r="D32" s="9"/>
+      <c r="E32" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="9">
-        <v>1</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="9"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
@@ -2481,13 +2536,13 @@
     </row>
     <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" s="9">
         <v>1</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E34" s="9"/>
     </row>
@@ -2498,7 +2553,7 @@
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -2530,22 +2585,30 @@
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="5"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="9">
+        <v>1</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" s="9"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
@@ -2583,7 +2646,7 @@
   <dimension ref="B2:E44"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2595,58 +2658,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -2812,147 +2875,151 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
+      <c r="C24" s="4">
+        <v>16</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C26" s="9">
         <v>1</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9" t="s">
+      <c r="D26" s="9"/>
+      <c r="E26" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C28" s="9">
         <v>1</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9" t="s">
+      <c r="D28" s="9"/>
+      <c r="E28" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C30" s="9">
         <v>1</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D30" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="9">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="9">
         <v>2</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9" t="s">
+      <c r="D31" s="9"/>
+      <c r="E31" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C33" s="9">
         <v>1</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D33" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" s="8" t="s">
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C35" s="9">
         <v>1</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D35" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="C35" s="9">
+      <c r="E35" s="9"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="9">
         <v>2</v>
       </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9" t="s">
+      <c r="D36" s="9"/>
+      <c r="E36" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="9">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="9">
         <v>1</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
-      <c r="C38" s="9">
+      <c r="D38" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="9"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="9">
         <v>2</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9" t="s">
+      <c r="D39" s="9"/>
+      <c r="E39" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
@@ -3002,7 +3069,7 @@
   <dimension ref="B2:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:E7"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3014,58 +3081,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -3105,7 +3172,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -3126,7 +3193,7 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -3193,71 +3260,71 @@
     </row>
     <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20" t="s">
-        <v>57</v>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
@@ -3322,10 +3389,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H39"/>
+  <dimension ref="B2:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3338,58 +3405,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -3419,7 +3486,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="E10" s="4"/>
     </row>
@@ -3429,7 +3496,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -3440,7 +3507,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -3521,57 +3588,57 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
@@ -3651,58 +3718,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -3742,7 +3809,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -3753,7 +3820,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -3834,57 +3901,57 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
@@ -3951,8 +4018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3964,58 +4031,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -4045,7 +4112,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E10" s="4"/>
     </row>
@@ -4055,7 +4122,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -4066,7 +4133,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -4147,57 +4214,57 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
@@ -4277,58 +4344,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -4348,7 +4415,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -4359,7 +4426,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -4368,7 +4435,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -4389,7 +4456,7 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -4398,7 +4465,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E14" s="4"/>
     </row>
@@ -4418,8 +4485,8 @@
         <v>8</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="18" t="s">
-        <v>73</v>
+      <c r="E16" s="11" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -4461,25 +4528,25 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="17" t="s">
-        <v>74</v>
+      <c r="B22" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="20">
+      <c r="C23" s="12">
         <v>2</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20" t="s">
-        <v>57</v>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -4489,25 +4556,25 @@
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="17" t="s">
-        <v>76</v>
+      <c r="B25" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="C25" s="9">
         <v>1</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
-      <c r="C26" s="20">
+      <c r="C26" s="12">
         <v>2</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20" t="s">
-        <v>57</v>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -4517,38 +4584,38 @@
       <c r="E27" s="6"/>
     </row>
     <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="s">
-        <v>78</v>
+      <c r="B28" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="C28" s="9">
         <v>1</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
-      <c r="C29" s="20">
+      <c r="C29" s="12">
         <v>2</v>
       </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20" t="s">
-        <v>80</v>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
@@ -4628,58 +4695,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="C4" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -4699,7 +4766,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -4710,7 +4777,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -4719,7 +4786,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -4740,7 +4807,7 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -4765,7 +4832,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
@@ -4806,74 +4873,74 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="17" t="s">
-        <v>86</v>
+      <c r="B22" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="20">
+      <c r="C23" s="12">
         <v>2</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20" t="s">
-        <v>57</v>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="17"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="17"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>

</xml_diff>

<commit_message>
update use case, especificação,relatorio
</commit_message>
<xml_diff>
--- a/2ª Fase/Diagramas/Especificaçao.xlsx
+++ b/2ª Fase/Diagramas/Especificaçao.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="8445" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="8445" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="Procurar restaurante" sheetId="1" r:id="rId1"/>
-    <sheet name="Procurar restaurante (teclado)" sheetId="3" r:id="rId2"/>
-    <sheet name="Procurar restaurante (voz)" sheetId="6" r:id="rId3"/>
-    <sheet name="Avaliar restaurante" sheetId="4" r:id="rId4"/>
-    <sheet name="Adicionar Restaurante aos fav" sheetId="7" r:id="rId5"/>
-    <sheet name="Partilhar Restaurante" sheetId="5" r:id="rId6"/>
-    <sheet name="Partilhar avaliação" sheetId="8" r:id="rId7"/>
-    <sheet name="Registar restaurante" sheetId="10" r:id="rId8"/>
-    <sheet name="Adicionar ementa" sheetId="11" r:id="rId9"/>
-    <sheet name="Editar ementa" sheetId="12" r:id="rId10"/>
-    <sheet name="Apagar ementa" sheetId="13" r:id="rId11"/>
+    <sheet name="Procurar produto - via teclado" sheetId="3" r:id="rId1"/>
+    <sheet name="Procurar produto - via voz" sheetId="6" r:id="rId2"/>
+    <sheet name="Procurar etiquetas favoritas" sheetId="14" r:id="rId3"/>
+    <sheet name="Selecionar Produto" sheetId="15" r:id="rId4"/>
+    <sheet name="Avaliar Produto" sheetId="4" r:id="rId5"/>
+    <sheet name="Adicionar Etiquetas favoritas" sheetId="7" r:id="rId6"/>
+    <sheet name="Partilhar Produtos" sheetId="5" r:id="rId7"/>
+    <sheet name="Partilhar avaliação" sheetId="8" r:id="rId8"/>
+    <sheet name="Registar restaurante" sheetId="10" r:id="rId9"/>
+    <sheet name="Adicionar ementa" sheetId="11" r:id="rId10"/>
+    <sheet name="Editar ementa" sheetId="12" r:id="rId11"/>
+    <sheet name="Apagar ementa" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -96,18 +97,9 @@
     <t>Especificação de Use Case</t>
   </si>
   <si>
-    <t>Carrega no botão</t>
-  </si>
-  <si>
     <t>Flow of events</t>
   </si>
   <si>
-    <t>Procura negócios num raio de 10km</t>
-  </si>
-  <si>
-    <t>Apresenta resultado obtidos</t>
-  </si>
-  <si>
     <t>Escolhe negócio a visitar</t>
   </si>
   <si>
@@ -135,253 +127,16 @@
     <t>Guarda informação</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Exceção 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (passo 3) [Não existe negócios num raio de 10km]</t>
-    </r>
-  </si>
-  <si>
     <t>Informa que não existe qualquer negócio perto do utilizador</t>
   </si>
   <si>
-    <t>Fecha a janela</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Comportamento Alternativo 1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(passo 4)</t>
-    </r>
-  </si>
-  <si>
-    <t>Volta para menu principal</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Comportamento Alternativo 2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(passo 6)</t>
-    </r>
-  </si>
-  <si>
-    <t>Procurar restaurante</t>
-  </si>
-  <si>
-    <t>Permite ao utilizador procurar um restaurante perto si, sem qualuqer restrição.</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Comportamento Alternativo 3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(passo 6)</t>
-    </r>
-  </si>
-  <si>
-    <t>Apresenta caixa de texto</t>
-  </si>
-  <si>
-    <t>Digita preferencias</t>
-  </si>
-  <si>
     <t>Valida dados</t>
   </si>
   <si>
-    <t>Permite ao utilizador procurar um restaurante perto si, sem qualquer restrição.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Exceção 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (passo 3) [Padrão de pesquisa errado]</t>
-    </r>
-  </si>
-  <si>
     <t>Indica que input é inválido</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Exceção 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (passo 4) [Não existe negócios num raio de 10km]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Comportamento Alternativo 1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(passo 7)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Comportamento Alternativo 2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(passo 9)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Comportamento Alternativo 3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(passo 9)</t>
-    </r>
-  </si>
-  <si>
-    <t>Recorrendo ao microfone, diz "Eat Up"</t>
-  </si>
-  <si>
-    <t>Reconhece sinal e mostra que está pronto a reconhecer</t>
-  </si>
-  <si>
-    <t>Cita preferencias</t>
   </si>
   <si>
     <r>
@@ -407,51 +162,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Exceção 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (passo 5) [Não existe negócios num raio de 10km]</t>
-    </r>
-  </si>
-  <si>
-    <t>Valida texto recebido por reconhecedor de voz</t>
-  </si>
-  <si>
-    <t>Procurar restaurante - com restrições (voz)</t>
-  </si>
-  <si>
-    <t>Procurar restaurante - com restrições (texto)</t>
-  </si>
-  <si>
-    <t>Avaliar estaurante</t>
-  </si>
-  <si>
-    <t>Permite ao utilizador avaliar um restaurante</t>
-  </si>
-  <si>
     <t>Utilizador autenticado</t>
-  </si>
-  <si>
-    <t>Visualiza histórico de negócios visitados</t>
-  </si>
-  <si>
-    <t>Escolhe negócio</t>
   </si>
   <si>
     <t>Guarda dados</t>
@@ -492,9 +203,6 @@
     <t>Partilhar restaurante</t>
   </si>
   <si>
-    <t>Adicionar restaurante aos favoritos</t>
-  </si>
-  <si>
     <t>Permite ao utilizador partilhar restaurante nas redes sociais</t>
   </si>
   <si>
@@ -504,9 +212,6 @@
     <t>Recorre a API da rede social a partilhar para publicar</t>
   </si>
   <si>
-    <t>Escolhe negócio anteriormente avaliado</t>
-  </si>
-  <si>
     <t>Registar restaurante</t>
   </si>
   <si>
@@ -633,10 +338,58 @@
     <t>Não confirma</t>
   </si>
   <si>
-    <t>Volta para 8</t>
-  </si>
-  <si>
-    <t>Seleciona etiqueta e adiciona aos favoritos</t>
+    <t>Preenche pontuação e critica</t>
+  </si>
+  <si>
+    <t>Procurar produto - via teclado</t>
+  </si>
+  <si>
+    <t>Permite a um cliente procurar um produto com as restrições desejadas.</t>
+  </si>
+  <si>
+    <t>Apresenta lista de negócios com o produto pretendido.</t>
+  </si>
+  <si>
+    <t>Carrega na opção procurar por teclado.</t>
+  </si>
+  <si>
+    <t>Apresenta caixa de texto.</t>
+  </si>
+  <si>
+    <t>Digita preferencias.</t>
+  </si>
+  <si>
+    <t>Seleciona raio de distancia pretendido.</t>
+  </si>
+  <si>
+    <t>Valida dados.</t>
+  </si>
+  <si>
+    <t>Procura negócios com preferencias indicadas.</t>
+  </si>
+  <si>
+    <t>Volta a 2.</t>
+  </si>
+  <si>
+    <t>Carrega na opção procurar por voz.</t>
+  </si>
+  <si>
+    <t>Confirma.</t>
+  </si>
+  <si>
+    <t>Procurar produto - via voz.</t>
+  </si>
+  <si>
+    <t>Mostra que esta pronto a reconhecer voz.</t>
+  </si>
+  <si>
+    <t>Cita preferencias.</t>
+  </si>
+  <si>
+    <t>Carrega na opção ver favoritos.</t>
+  </si>
+  <si>
+    <t>Apresenta lista com favoritos.</t>
   </si>
   <si>
     <r>
@@ -648,7 +401,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Comportamento Alternativo 4 </t>
+      <t>Exceção 2</t>
     </r>
     <r>
       <rPr>
@@ -658,11 +411,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(passo 16)</t>
+      <t xml:space="preserve"> (passo 7) [Não existe negócios no raio indicado]</t>
     </r>
   </si>
   <si>
-    <t>Volta para 16</t>
+    <t>Escolhe etiquetas pretendidas.</t>
   </si>
   <si>
     <r>
@@ -674,7 +427,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Comportamento Alternativo 3 </t>
+      <t>Exceção 1</t>
     </r>
     <r>
       <rPr>
@@ -684,14 +437,141 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(passo 16)</t>
+      <t xml:space="preserve"> (passo 3) [Utilizador não  tem etiquetas favoritas]</t>
     </r>
   </si>
   <si>
-    <t>Preenche pontuação e critica</t>
-  </si>
-  <si>
-    <t>Escolhe negócio e ementa consumida</t>
+    <t>Indica que utilizador não tem etiquetas favoritas.</t>
+  </si>
+  <si>
+    <t>Volta a menu principal.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exceção 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (passo 6) [Padrão de pesquisa errado]</t>
+    </r>
+  </si>
+  <si>
+    <t>Apresenta resultados obtidos com as ementas que correspondem bem como os negócios e as suas distancias.</t>
+  </si>
+  <si>
+    <t>Selecionar restaurantes.</t>
+  </si>
+  <si>
+    <t>Procura efetuada.</t>
+  </si>
+  <si>
+    <t>Ementa registada no histórico.</t>
+  </si>
+  <si>
+    <t>Permite ao cliente selecionar restaurantes da pesquisa.</t>
+  </si>
+  <si>
+    <t>Seleciona um dos resultados</t>
+  </si>
+  <si>
+    <t>Calcula rota mais breve.</t>
+  </si>
+  <si>
+    <t>Apresenta rota em mapa.</t>
+  </si>
+  <si>
+    <t>Marca como visitado.</t>
+  </si>
+  <si>
+    <t>Guarda dados.</t>
+  </si>
+  <si>
+    <t>Volta para menu principal.</t>
+  </si>
+  <si>
+    <t>Seleciona navegação.</t>
+  </si>
+  <si>
+    <t>Apresenta navegação GPS.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Comportamento Alternativo 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (4) [Dispositivo não tem GPS]</t>
+    </r>
+  </si>
+  <si>
+    <t>Passa para 6.</t>
+  </si>
+  <si>
+    <t>Avaliar produto.</t>
+  </si>
+  <si>
+    <t>Permite ao utilizador avaliar um produto.</t>
+  </si>
+  <si>
+    <t>Produto avaliada.</t>
+  </si>
+  <si>
+    <t>Visualiza histórico de produtos.</t>
+  </si>
+  <si>
+    <t>Escolhe produto.</t>
+  </si>
+  <si>
+    <t>Adicionar etiquetas favoritas.</t>
+  </si>
+  <si>
+    <t>Seleciona adicionar etiquetas.</t>
+  </si>
+  <si>
+    <t>Mostra caixa de texto.</t>
+  </si>
+  <si>
+    <t>Escreve etiquetas.</t>
+  </si>
+  <si>
+    <t>Partilhar produtos.</t>
+  </si>
+  <si>
+    <t>Permite ao utilizador partilhar ementa nas redes sociais</t>
+  </si>
+  <si>
+    <t>Visualiza historico de avaliações.</t>
+  </si>
+  <si>
+    <t>Escolhe avaliação a partilhar.</t>
   </si>
 </sst>
 </file>
@@ -741,7 +621,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -841,11 +721,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -908,6 +810,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1190,10 +1099,346 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K25"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="B18:E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="50" customWidth="1"/>
+    <col min="5" max="5" width="56.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="4">
+        <v>7</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="4">
+        <v>4</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="4">
+        <v>8</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="4">
+        <v>9</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="4">
+        <v>6</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="4">
+        <v>10</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="4">
+        <v>7</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="4">
+        <v>11</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="4">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="4">
+        <v>12</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="4">
+        <v>13</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="4">
+        <v>14</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="4">
+        <v>15</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="4">
+        <v>16</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="4">
+        <v>17</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="4">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
@@ -1233,7 +1478,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
@@ -1243,7 +1488,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
@@ -1253,14 +1498,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -1276,7 +1521,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -1287,7 +1532,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -1295,20 +1540,20 @@
       <c r="C11" s="4">
         <v>3</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="D11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="4">
         <v>4</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
@@ -1317,7 +1562,7 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -1325,9 +1570,7 @@
       <c r="C14" s="4">
         <v>6</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1336,9 +1579,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
@@ -1346,18 +1587,14 @@
         <v>8</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="4">
         <v>9</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -1366,18 +1603,14 @@
         <v>10</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="4">
         <v>11</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -1386,9 +1619,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
@@ -1397,118 +1628,86 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
-        <v>20</v>
+      <c r="B22" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="9">
-        <v>1</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="9"/>
+      <c r="C23" s="12">
+        <v>2</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="9">
-        <v>2</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="9">
-        <v>1</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="9"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="9">
-        <v>1</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
-      <c r="C30" s="9">
-        <v>2</v>
-      </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="9">
-        <v>1</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
-      <c r="C33" s="9">
-        <v>2</v>
-      </c>
+      <c r="C33" s="9"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
@@ -1550,16 +1749,16 @@
   <mergeCells count="5">
     <mergeCell ref="B2:E3"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C7:E7"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E39"/>
   <sheetViews>
@@ -1594,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
@@ -1604,7 +1803,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
@@ -1614,7 +1813,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
@@ -1624,14 +1823,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -1647,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -1658,7 +1857,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -1667,7 +1866,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -1678,7 +1877,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -1687,7 +1886,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="E13" s="4"/>
     </row>
@@ -1698,7 +1897,7 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1708,7 +1907,7 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -1759,14 +1958,14 @@
     </row>
     <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1776,7 +1975,7 @@
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -1888,7 +2087,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E39"/>
   <sheetViews>
@@ -1923,7 +2122,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
@@ -1933,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
@@ -1943,7 +2142,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
@@ -1953,14 +2152,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -1976,7 +2175,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -1987,7 +2186,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -1996,7 +2195,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -2007,7 +2206,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -2016,7 +2215,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="E13" s="4"/>
     </row>
@@ -2027,7 +2226,7 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -2085,13 +2284,13 @@
     </row>
     <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="E22" s="9"/>
     </row>
@@ -2102,7 +2301,7 @@
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -2216,10 +2415,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E44"/>
+  <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,7 +2448,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
@@ -2259,7 +2458,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
@@ -2269,7 +2468,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
@@ -2279,14 +2478,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -2302,7 +2501,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -2313,7 +2512,7 @@
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -2322,7 +2521,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E11" s="9"/>
     </row>
@@ -2331,29 +2530,29 @@
       <c r="C12" s="4">
         <v>4</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="D12" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="4">
         <v>5</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="D13" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="4">
         <v>6</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
-        <v>10</v>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -2361,272 +2560,94 @@
       <c r="C15" s="4">
         <v>7</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="4">
         <v>8</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="4" t="s">
-        <v>12</v>
+      <c r="E16" s="11" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
-      <c r="C17" s="4">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="4">
-        <v>10</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
-        <v>14</v>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="4">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="4">
-        <v>12</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="4">
-        <v>13</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="4">
-        <v>14</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="C23" s="4">
-        <v>15</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="4">
-        <v>16</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
-      <c r="C25" s="4">
-        <v>17</v>
-      </c>
+      <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="9">
-        <v>1</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="9">
-        <v>1</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="9">
-        <v>1</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="9">
-        <v>2</v>
-      </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="9">
-        <v>1</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="C35" s="9">
-        <v>2</v>
-      </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="9">
-        <v>1</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
-      <c r="C38" s="9">
-        <v>2</v>
-      </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40" s="9">
-        <v>1</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="5"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="5"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="5"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="5"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2643,21 +2664,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E44"/>
+  <dimension ref="B2:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
     <col min="5" max="5" width="56.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" customWidth="1"/>
+    <col min="10" max="10" width="31.5703125" customWidth="1"/>
+    <col min="11" max="11" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
         <v>6</v>
       </c>
@@ -2665,55 +2690,55 @@
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -2723,333 +2748,245 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="4">
         <v>2</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="4">
         <v>3</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="H11" s="5"/>
+      <c r="I11" s="4">
+        <v>7</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="4">
         <v>4</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="4">
+        <v>8</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="4">
         <v>5</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9" t="s">
+      <c r="D13" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="4">
         <v>6</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="4">
         <v>7</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="4">
         <v>11</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J15" s="4"/>
+      <c r="K15" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="4">
         <v>8</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
-      <c r="C17" s="4">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="4">
         <v>13</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="4">
-        <v>10</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
+      <c r="J17" s="4"/>
+      <c r="K17" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="4">
+        <v>14</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="4">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J19" s="4"/>
+      <c r="K19" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="4">
-        <v>12</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="4">
         <v>16</v>
       </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="4">
+      <c r="J20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4" t="s">
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="H21" s="5"/>
+      <c r="I21" s="4">
+        <v>17</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="4">
-        <v>14</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="C23" s="4">
-        <v>15</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="4">
-        <v>16</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="9">
-        <v>1</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="9">
-        <v>1</v>
-      </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="9">
-        <v>1</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="9">
-        <v>2</v>
-      </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="9">
-        <v>1</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B35" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="9">
-        <v>1</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="9"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="C36" s="9">
-        <v>2</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C38" s="9">
-        <v>1</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="E38" s="9"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-      <c r="C39" s="9">
-        <v>2</v>
-      </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="5"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="5"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="5"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="5"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="5"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3066,10 +3003,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E39"/>
+  <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K29" sqref="K28:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3086,20 +3023,20 @@
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
@@ -3109,7 +3046,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
@@ -3119,7 +3056,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
@@ -3129,14 +3066,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -3152,7 +3089,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -3161,39 +3098,39 @@
       <c r="C10" s="4">
         <v>2</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="4"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="4">
         <v>3</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="4">
         <v>4</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="D12" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="4">
         <v>5</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>53</v>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -3201,178 +3138,92 @@
       <c r="C14" s="4">
         <v>6</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="D14" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="22"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="4">
         <v>7</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="4">
         <v>8</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
-      <c r="C17" s="4">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="4">
-        <v>10</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="4">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="4">
-        <v>12</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="9">
-        <v>1</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="5"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="5"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="5"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3392,7 +3243,7 @@
   <dimension ref="B2:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B22" sqref="B22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3401,7 +3252,6 @@
     <col min="3" max="3" width="6.5703125" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
     <col min="5" max="5" width="56.7109375" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
@@ -3423,7 +3273,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
@@ -3433,7 +3283,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
@@ -3443,7 +3293,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
@@ -3453,14 +3303,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -3476,7 +3326,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -3486,7 +3336,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E10" s="4"/>
     </row>
@@ -3496,7 +3346,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -3507,7 +3357,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -3516,7 +3366,9 @@
         <v>5</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
@@ -3580,17 +3432,25 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
+    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1</v>
+      </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
@@ -3706,7 +3566,7 @@
   <dimension ref="B2:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3715,6 +3575,7 @@
     <col min="3" max="3" width="6.5703125" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
     <col min="5" max="5" width="56.7109375" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
@@ -3736,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
@@ -3746,7 +3607,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
@@ -3756,7 +3617,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
@@ -3766,14 +3627,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -3789,7 +3650,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -3798,10 +3659,10 @@
       <c r="C10" s="4">
         <v>2</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
@@ -3809,7 +3670,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -3820,7 +3681,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -3829,7 +3690,9 @@
         <v>5</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
@@ -3893,17 +3756,27 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
+    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1</v>
+      </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
@@ -4018,8 +3891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4049,7 +3922,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
@@ -4059,7 +3932,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
@@ -4069,7 +3942,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
@@ -4079,14 +3952,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -4102,7 +3975,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -4112,7 +3985,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="E10" s="4"/>
     </row>
@@ -4122,7 +3995,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -4133,7 +4006,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -4328,6 +4201,319 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="50" customWidth="1"/>
+    <col min="5" max="5" width="56.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="4">
+        <v>4</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="4">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="4">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="4">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="4">
+        <v>9</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="4">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="4">
+        <v>11</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="4">
+        <v>12</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E39"/>
   <sheetViews>
@@ -4362,7 +4548,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
@@ -4372,7 +4558,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
@@ -4382,7 +4568,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
@@ -4392,14 +4578,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -4415,7 +4601,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -4426,7 +4612,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -4435,7 +4621,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -4446,7 +4632,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -4456,7 +4642,7 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -4465,7 +4651,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="E14" s="4"/>
     </row>
@@ -4476,7 +4662,7 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -4486,7 +4672,7 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="11" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -4529,14 +4715,14 @@
     </row>
     <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -4546,7 +4732,7 @@
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -4557,14 +4743,14 @@
     </row>
     <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="C25" s="9">
         <v>1</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -4574,7 +4760,7 @@
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -4585,14 +4771,14 @@
     </row>
     <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C28" s="9">
         <v>1</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -4602,333 +4788,8 @@
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="5"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="5"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="5"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="4">
-        <v>2</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="4">
-        <v>3</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="4">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="4">
-        <v>5</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="4">
-        <v>6</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="4">
-        <v>7</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="4">
-        <v>8</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="4">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="4">
-        <v>10</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="4">
-        <v>11</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="4">
-        <v>12</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="9">
-        <v>1</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="12">
-        <v>2</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>

</xml_diff>